<commit_message>
Bug:faltaban datos al descargar el excel
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/parameter/ParameterFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/parameter/ParameterFormulario.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ReposAxsis\API\Service.Catalog\wwwroot\layout\excel\parameter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE4CFEC-FD22-426C-A4C5-91853CB2D621}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C0FEC3-485A-46A2-B48C-DF8C3E5B50EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="Estudios">Parameter!$A$21:$B$22</definedName>
     <definedName name="Parameter" localSheetId="0">Parameter!$A$3:$F$19</definedName>
+    <definedName name="TiposVAlor">Parameter!$D$23:$R$24</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Clave</t>
   </si>
@@ -111,46 +114,148 @@
     <t>FCSI</t>
   </si>
   <si>
-    <t>{{Parameter.clave}}</t>
-  </si>
-  <si>
-    <t>{{Parameter.nombre}}</t>
-  </si>
-  <si>
-    <t>{{Parameter.nombreCorto}}</t>
-  </si>
-  <si>
-    <t>{{Parameter.unidades}}</t>
-  </si>
-  <si>
-    <t>{{Parameter.tipoValor}}</t>
-  </si>
-  <si>
-    <t>{{Parameter.format.Nombre}}</t>
-  </si>
-  <si>
-    <t>{{Parameter.formato}}</t>
-  </si>
-  <si>
-    <t>{{Parameter.valorInicial}}</t>
-  </si>
-  <si>
-    <t>{{Parameter.areas.Departamneto.Nombre}}</t>
-  </si>
-  <si>
-    <t>{{Parameter.areas.Nombre}}</t>
-  </si>
-  <si>
-    <t>{{Parameter.reactivos.Nombre}}</t>
-  </si>
-  <si>
-    <t>{{Parameter.unidadSi}}</t>
-  </si>
-  <si>
-    <t>{{Parameter.fcs}}</t>
-  </si>
-  <si>
     <t>{{Parameter.activo}}</t>
+  </si>
+  <si>
+    <t>Estudios</t>
+  </si>
+  <si>
+    <t>{{item.Id}}</t>
+  </si>
+  <si>
+    <t>{{item.Nombre}}</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>valorInicial</t>
+  </si>
+  <si>
+    <t>valorFinal</t>
+  </si>
+  <si>
+    <t>valorInicialNumerico</t>
+  </si>
+  <si>
+    <t>valorFinalNumerico</t>
+  </si>
+  <si>
+    <t>rangoEdadInicial</t>
+  </si>
+  <si>
+    <t>rangoEdadFinal</t>
+  </si>
+  <si>
+    <t>hombreValorInicial</t>
+  </si>
+  <si>
+    <t>hombreValorFinal</t>
+  </si>
+  <si>
+    <t>mujerValorInicial</t>
+  </si>
+  <si>
+    <t>mujerValorFinal</t>
+  </si>
+  <si>
+    <t>medidaTiempo</t>
+  </si>
+  <si>
+    <t>opcion</t>
+  </si>
+  <si>
+    <t>descripcionTexto</t>
+  </si>
+  <si>
+    <t>descripcionParrafo</t>
+  </si>
+  <si>
+    <t>Valores</t>
+  </si>
+  <si>
+    <t>{{item.nombre}}</t>
+  </si>
+  <si>
+    <t>{{item.valorInicial}}</t>
+  </si>
+  <si>
+    <t>{{item.valorFinal}}</t>
+  </si>
+  <si>
+    <t>{{item.valorInicialNumerico}}</t>
+  </si>
+  <si>
+    <t>{{item.valorFinalNumerico}}</t>
+  </si>
+  <si>
+    <t>{{item.rangoEdadInicial}}</t>
+  </si>
+  <si>
+    <t>{{item.rangoEdadFinal}}</t>
+  </si>
+  <si>
+    <t>{{item.hombreValorInicial}}</t>
+  </si>
+  <si>
+    <t>{{item.hombreValorFinal}}</t>
+  </si>
+  <si>
+    <t>{{item.mujerValorInicial}}</t>
+  </si>
+  <si>
+    <t>{{item.mujerValorFinal}}</t>
+  </si>
+  <si>
+    <t>{{item.medidaTiempo}}</t>
+  </si>
+  <si>
+    <t>{{item.opcion}}</t>
+  </si>
+  <si>
+    <t>{{item.descripcionTexto}}</t>
+  </si>
+  <si>
+    <t>{{item.descripcionParrafo}}</t>
+  </si>
+  <si>
+    <t>{{Parameter.Clave}}</t>
+  </si>
+  <si>
+    <t>{{Parameter.Nombre}}</t>
+  </si>
+  <si>
+    <t>{{Parameter.NombreCorto}}</t>
+  </si>
+  <si>
+    <t>{{Parameter.Unidades}}</t>
+  </si>
+  <si>
+    <t>{{Parameter.TipoValor}}</t>
+  </si>
+  <si>
+    <t>{{Parameter.Format.Nombre}}</t>
+  </si>
+  <si>
+    <t>{{Parameter.Formato}}</t>
+  </si>
+  <si>
+    <t>{{Parameter.ValorInicial}}</t>
+  </si>
+  <si>
+    <t>{{Parameter.Areas.Departamento.Nombre}}</t>
+  </si>
+  <si>
+    <t>{{Parameter.Areas.Nombre}}</t>
+  </si>
+  <si>
+    <t>{{Parameter.Reactivos.Nombre}}</t>
+  </si>
+  <si>
+    <t>{{Parameter.UnidadSi}}</t>
+  </si>
+  <si>
+    <t>{{Parameter.Fcsi}}</t>
   </si>
 </sst>
 </file>
@@ -217,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -231,11 +336,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -606,23 +717,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A4281-45E9-4A26-88B5-8DB32AE336F4}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:F13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="30.7109375" customWidth="1"/>
+    <col min="1" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
@@ -630,17 +758,17 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="5"/>
+      <c r="B3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="8"/>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="5"/>
+      <c r="E3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -651,17 +779,17 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="5"/>
+      <c r="B5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="8"/>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="5"/>
+      <c r="E5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -672,17 +800,17 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="5"/>
+      <c r="B7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="8"/>
       <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="5"/>
+      <c r="E7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -693,17 +821,17 @@
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="5"/>
+      <c r="B9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="8"/>
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="5"/>
+      <c r="E9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -714,17 +842,17 @@
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="5"/>
+      <c r="B11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="8"/>
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="5"/>
+      <c r="E11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -735,17 +863,17 @@
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="5"/>
+      <c r="B13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="8"/>
       <c r="D13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="5"/>
+      <c r="E13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -756,7 +884,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="1"/>
@@ -765,40 +893,170 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="5"/>
+      <c r="B17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="8"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="5"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="5"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="R21" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D23" s="1"/>
-      <c r="E23" s="2"/>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" t="s">
+        <v>41</v>
+      </c>
+      <c r="K23" t="s">
+        <v>42</v>
+      </c>
+      <c r="L23" t="s">
+        <v>43</v>
+      </c>
+      <c r="M23" t="s">
+        <v>44</v>
+      </c>
+      <c r="N23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O23" t="s">
+        <v>46</v>
+      </c>
+      <c r="P23" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>48</v>
+      </c>
+      <c r="R23" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="35">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E5:F5"/>
@@ -808,14 +1066,42 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N20:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62E81AE-DE66-4B86-8915-482BEECB9B24}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Parámetros - BUG Al editar un tipo de valor, solo debería aparecer un mensaje correspondiente a la acción.
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/parameter/ParameterFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/parameter/ParameterFormulario.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ReposAxsis\API\Service.Catalog\wwwroot\layout\excel\parameter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ResposAxsis\API\Service.Catalog\wwwroot\layout\excel\parameter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77701D6-C555-45FD-AD28-BF1C6E240ABA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <definedName name="Parameter" localSheetId="0">Parameter!$A$3:$F$19</definedName>
     <definedName name="TiposVAlor">Parameter!$D$23:$R$24</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -207,18 +206,6 @@
     <t>{{item.mujerValorFinal}}</t>
   </si>
   <si>
-    <t>{{item.medidaTiempo}}</t>
-  </si>
-  <si>
-    <t>{{item.opcion}}</t>
-  </si>
-  <si>
-    <t>{{item.descripcionTexto}}</t>
-  </si>
-  <si>
-    <t>{{item.descripcionParrafo}}</t>
-  </si>
-  <si>
     <t>{{Parameter.Clave}}</t>
   </si>
   <si>
@@ -256,12 +243,24 @@
   </si>
   <si>
     <t>{{Parameter.Format}}</t>
+  </si>
+  <si>
+    <t>{{item.DescripcionTexto}}</t>
+  </si>
+  <si>
+    <t>{{item.DescripcionParrafo}}</t>
+  </si>
+  <si>
+    <t>{{item.Opcion}}</t>
+  </si>
+  <si>
+    <t>{{item.MedidaTiempoId}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -322,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -339,14 +338,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,11 +718,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A4281-45E9-4A26-88B5-8DB32AE336F4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C13"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,11 +748,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
@@ -758,17 +760,17 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="6"/>
+      <c r="B3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="9"/>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="6"/>
+      <c r="E3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -779,17 +781,17 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="6"/>
+      <c r="B5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="9"/>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="6"/>
+      <c r="E5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -800,17 +802,17 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="6"/>
+      <c r="B7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="9"/>
       <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" s="6"/>
+      <c r="E7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -821,17 +823,17 @@
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="6"/>
+      <c r="B9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="9"/>
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="6"/>
+      <c r="E9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -842,17 +844,17 @@
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="6"/>
+      <c r="B11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="9"/>
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="6"/>
+      <c r="E11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -863,17 +865,17 @@
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="6"/>
+      <c r="B13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="9"/>
       <c r="D13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -884,7 +886,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="1"/>
@@ -897,10 +899,10 @@
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="6"/>
+      <c r="B17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="9"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
@@ -908,43 +910,43 @@
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8" t="s">
+      <c r="B19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
       <c r="R19" s="5"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
       <c r="R20" s="5"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -954,46 +956,46 @@
       <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L21" s="8" t="s">
+      <c r="L21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M21" s="8" t="s">
+      <c r="M21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N21" s="8" t="s">
+      <c r="N21" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O21" s="8" t="s">
+      <c r="O21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="P21" s="8" t="s">
+      <c r="P21" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Q21" s="8" t="s">
+      <c r="Q21" s="6" t="s">
         <v>32</v>
       </c>
       <c r="R21" s="5" t="s">
@@ -1038,41 +1040,25 @@
         <v>45</v>
       </c>
       <c r="O23" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="P23" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="Q23" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="R23" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="A19:B19"/>
+  <mergeCells count="28">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E5:F5"/>
@@ -1082,11 +1068,20 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N20:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1095,7 +1090,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62E81AE-DE66-4B86-8915-482BEECB9B24}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>